<commit_message>
Added Students tests and some improvements
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Тесты</t>
   </si>
@@ -113,6 +113,42 @@
   </si>
   <si>
     <t>Can_Filter_Courses</t>
+  </si>
+  <si>
+    <t>Переход к Students</t>
+  </si>
+  <si>
+    <t>Создание Students</t>
+  </si>
+  <si>
+    <t>Удаление Students</t>
+  </si>
+  <si>
+    <t>Поиск Students</t>
+  </si>
+  <si>
+    <t>Редактирование Students</t>
+  </si>
+  <si>
+    <t>Can_Search_Students</t>
+  </si>
+  <si>
+    <t>Can_Navigate_To_Students</t>
+  </si>
+  <si>
+    <t>Can_Create_Students</t>
+  </si>
+  <si>
+    <t>Can_Delete_Students</t>
+  </si>
+  <si>
+    <t>Can_Edit_Student</t>
+  </si>
+  <si>
+    <t>Переход к Student Body Statistics</t>
+  </si>
+  <si>
+    <t>Can_Navigate_To_About</t>
   </si>
 </sst>
 </file>
@@ -456,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,25 +670,91 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C24">
+      <c r="C26">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C25">
+      <c r="C27">
         <v>1</v>
       </c>
     </row>

</xml_diff>